<commit_message>
Millennial calibrated and run for LRF
</commit_message>
<xml_diff>
--- a/Millennial/R/simulation/LRF/Calibration tests_LRF.xlsx
+++ b/Millennial/R/simulation/LRF/Calibration tests_LRF.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\edmaas\Documents\Modeling\Millennial\R\simulation\LRF\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDBCC905-E048-48F4-913D-54839CDA4FC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7567018-BF05-4808-BB00-EC5DF371F5C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{BB3C2B61-1532-46D1-807E-A73843A0FCA4}"/>
+    <workbookView xWindow="34635" yWindow="3780" windowWidth="18540" windowHeight="9765" xr2:uid="{BB3C2B61-1532-46D1-807E-A73843A0FCA4}"/>
   </bookViews>
   <sheets>
     <sheet name="1_3" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="21">
   <si>
     <t>SOC 1850</t>
   </si>
@@ -70,9 +70,6 @@
     <t>derivs_V2_MM</t>
   </si>
   <si>
-    <t>derivs_V2_ECA</t>
-  </si>
-  <si>
     <t>1_2</t>
   </si>
   <si>
@@ -89,6 +86,18 @@
   </si>
   <si>
     <t>SOC 2003</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>Default for model V2 paper, using Fit Values: All</t>
+  </si>
+  <si>
+    <t>Fit values for VR dataset (Australian sites)</t>
+  </si>
+  <si>
+    <t>Goal is 72 in 1940 to 44 in 2003 (diff = 27.6)</t>
   </si>
 </sst>
 </file>
@@ -461,11 +470,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8287DD4-9EE1-45C0-9DA6-CB950E61C7F6}">
-  <dimension ref="A1:L49"/>
+  <dimension ref="A1:M50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K2" sqref="K2"/>
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I27" sqref="I27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -480,7 +489,7 @@
     <col min="8" max="8" width="6.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>8</v>
       </c>
@@ -494,10 +503,10 @@
         <v>2</v>
       </c>
       <c r="E1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G1" t="s">
         <v>5</v>
@@ -509,21 +518,24 @@
         <v>7</v>
       </c>
       <c r="J1" t="s">
+        <v>15</v>
+      </c>
+      <c r="K1" t="s">
         <v>16</v>
-      </c>
-      <c r="K1" t="s">
-        <v>17</v>
       </c>
       <c r="L1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="M1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -546,26 +558,534 @@
       <c r="I2">
         <v>0</v>
       </c>
+      <c r="J2">
+        <v>55</v>
+      </c>
+      <c r="K2">
+        <v>60</v>
+      </c>
       <c r="L2">
         <f>J2-K2</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A48"/>
-      <c r="B48"/>
-      <c r="C48"/>
-      <c r="D48"/>
-      <c r="E48"/>
-      <c r="F48"/>
-      <c r="G48"/>
-      <c r="H48"/>
-      <c r="I48"/>
-      <c r="J48"/>
-      <c r="K48"/>
-      <c r="L48"/>
-    </row>
-    <row r="49" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.35">
+        <v>-5</v>
+      </c>
+      <c r="M2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3">
+        <v>8617</v>
+      </c>
+      <c r="E3">
+        <v>1.5E-3</v>
+      </c>
+      <c r="F3">
+        <v>774.6</v>
+      </c>
+      <c r="G3">
+        <v>0.19</v>
+      </c>
+      <c r="H3">
+        <v>1.2E-2</v>
+      </c>
+      <c r="J3">
+        <v>78</v>
+      </c>
+      <c r="K3">
+        <v>80</v>
+      </c>
+      <c r="L3">
+        <f>J3-K3</f>
+        <v>-2</v>
+      </c>
+      <c r="M3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4">
+        <v>3</v>
+      </c>
+      <c r="D4">
+        <v>6443</v>
+      </c>
+      <c r="E4">
+        <v>1.5E-3</v>
+      </c>
+      <c r="F4">
+        <v>290</v>
+      </c>
+      <c r="G4">
+        <v>0.6</v>
+      </c>
+      <c r="H4">
+        <v>1.2E-2</v>
+      </c>
+      <c r="J4">
+        <v>27</v>
+      </c>
+      <c r="K4">
+        <v>3.2</v>
+      </c>
+      <c r="L4">
+        <f>J4-K4</f>
+        <v>23.8</v>
+      </c>
+      <c r="M4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="C5">
+        <v>4</v>
+      </c>
+      <c r="D5">
+        <v>5000</v>
+      </c>
+      <c r="J5">
+        <v>22.4</v>
+      </c>
+      <c r="K5">
+        <v>2.4</v>
+      </c>
+      <c r="L5">
+        <f t="shared" ref="L5:L27" si="0">J5-K5</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="C6">
+        <v>5</v>
+      </c>
+      <c r="D6">
+        <v>8617</v>
+      </c>
+      <c r="J6">
+        <v>33.799999999999997</v>
+      </c>
+      <c r="K6">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="L6">
+        <f t="shared" si="0"/>
+        <v>29.4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="C7">
+        <v>6</v>
+      </c>
+      <c r="F7">
+        <v>400</v>
+      </c>
+      <c r="J7">
+        <v>37</v>
+      </c>
+      <c r="K7">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="L7">
+        <f t="shared" si="0"/>
+        <v>32.1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="C8">
+        <v>7</v>
+      </c>
+      <c r="G8">
+        <v>0.5</v>
+      </c>
+      <c r="J8">
+        <v>36.9</v>
+      </c>
+      <c r="K8">
+        <v>5.6</v>
+      </c>
+      <c r="L8">
+        <f t="shared" si="0"/>
+        <v>31.299999999999997</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="C9">
+        <v>8</v>
+      </c>
+      <c r="F9">
+        <v>600</v>
+      </c>
+      <c r="J9">
+        <v>43.6</v>
+      </c>
+      <c r="K9">
+        <v>6.7</v>
+      </c>
+      <c r="L9">
+        <f t="shared" si="0"/>
+        <v>36.9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="C10">
+        <v>9</v>
+      </c>
+      <c r="F10">
+        <v>700</v>
+      </c>
+      <c r="G10">
+        <v>0.3</v>
+      </c>
+      <c r="J10">
+        <v>57.7</v>
+      </c>
+      <c r="K10">
+        <v>15.8</v>
+      </c>
+      <c r="L10">
+        <f t="shared" si="0"/>
+        <v>41.900000000000006</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="C11">
+        <v>10</v>
+      </c>
+      <c r="F11">
+        <v>800</v>
+      </c>
+      <c r="G11">
+        <v>0.5</v>
+      </c>
+      <c r="J11">
+        <v>50.3</v>
+      </c>
+      <c r="K11">
+        <v>7.8</v>
+      </c>
+      <c r="L11">
+        <f t="shared" si="0"/>
+        <v>42.5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="C12">
+        <v>11</v>
+      </c>
+      <c r="G12">
+        <v>0.2</v>
+      </c>
+      <c r="J12">
+        <v>77</v>
+      </c>
+      <c r="K12">
+        <v>68</v>
+      </c>
+      <c r="L12">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="C13">
+        <v>12</v>
+      </c>
+      <c r="G13">
+        <v>0.3</v>
+      </c>
+      <c r="J13">
+        <v>62.5</v>
+      </c>
+      <c r="K13">
+        <v>17.2</v>
+      </c>
+      <c r="L13">
+        <f t="shared" si="0"/>
+        <v>45.3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="C14">
+        <v>13</v>
+      </c>
+      <c r="G14">
+        <v>0.25</v>
+      </c>
+      <c r="J14">
+        <v>68.8</v>
+      </c>
+      <c r="K14">
+        <v>27.4</v>
+      </c>
+      <c r="L14">
+        <f t="shared" si="0"/>
+        <v>41.4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="C15">
+        <v>14</v>
+      </c>
+      <c r="G15">
+        <v>0.27500000000000002</v>
+      </c>
+      <c r="J15">
+        <v>65.400000000000006</v>
+      </c>
+      <c r="K15">
+        <v>21.1</v>
+      </c>
+      <c r="L15">
+        <f t="shared" si="0"/>
+        <v>44.300000000000004</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="C16">
+        <v>15</v>
+      </c>
+      <c r="G16">
+        <v>0.22500000000000001</v>
+      </c>
+      <c r="J16">
+        <v>72.900000000000006</v>
+      </c>
+      <c r="K16">
+        <v>39.5</v>
+      </c>
+      <c r="L16">
+        <f t="shared" si="0"/>
+        <v>33.400000000000006</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="C17">
+        <v>16</v>
+      </c>
+      <c r="G17">
+        <v>0.215</v>
+      </c>
+      <c r="J17">
+        <v>74.7</v>
+      </c>
+      <c r="K17">
+        <v>48.1</v>
+      </c>
+      <c r="L17">
+        <f t="shared" si="0"/>
+        <v>26.6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="C18">
+        <v>17</v>
+      </c>
+      <c r="F18">
+        <v>850</v>
+      </c>
+      <c r="J18">
+        <v>77.7</v>
+      </c>
+      <c r="K18">
+        <v>50.6</v>
+      </c>
+      <c r="L18">
+        <f t="shared" si="0"/>
+        <v>27.1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="C19">
+        <v>18</v>
+      </c>
+      <c r="D19">
+        <v>8200</v>
+      </c>
+      <c r="F19">
+        <v>875</v>
+      </c>
+      <c r="J19">
+        <v>76</v>
+      </c>
+      <c r="K19">
+        <v>49.6</v>
+      </c>
+      <c r="L19">
+        <f t="shared" si="0"/>
+        <v>26.4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="C20">
+        <v>19</v>
+      </c>
+      <c r="G20">
+        <v>0.22500000000000001</v>
+      </c>
+      <c r="J20">
+        <v>74</v>
+      </c>
+      <c r="K20">
+        <v>40.5</v>
+      </c>
+      <c r="L20">
+        <f t="shared" si="0"/>
+        <v>33.5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="C21">
+        <v>20</v>
+      </c>
+      <c r="D21">
+        <v>8000</v>
+      </c>
+      <c r="J21">
+        <v>72.599999999999994</v>
+      </c>
+      <c r="K21">
+        <v>39.6</v>
+      </c>
+      <c r="L21">
+        <f t="shared" si="0"/>
+        <v>32.999999999999993</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="C22">
+        <v>21</v>
+      </c>
+      <c r="D22">
+        <v>8200</v>
+      </c>
+      <c r="G22">
+        <v>0.215</v>
+      </c>
+      <c r="J22">
+        <v>76</v>
+      </c>
+      <c r="K22">
+        <v>49.6</v>
+      </c>
+      <c r="L22">
+        <f t="shared" si="0"/>
+        <v>26.4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="C23">
+        <v>22</v>
+      </c>
+      <c r="D23">
+        <v>8000</v>
+      </c>
+      <c r="J23">
+        <v>74.400000000000006</v>
+      </c>
+      <c r="K23">
+        <v>48.5</v>
+      </c>
+      <c r="L23">
+        <f t="shared" si="0"/>
+        <v>25.900000000000006</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="C24">
+        <v>23</v>
+      </c>
+      <c r="G24">
+        <v>0.22</v>
+      </c>
+      <c r="J24">
+        <v>73.5</v>
+      </c>
+      <c r="K24">
+        <v>43.5</v>
+      </c>
+      <c r="L24">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="C25">
+        <v>24</v>
+      </c>
+      <c r="G25">
+        <v>0.218</v>
+      </c>
+      <c r="J25">
+        <v>73.900000000000006</v>
+      </c>
+      <c r="K25">
+        <v>45.4</v>
+      </c>
+      <c r="L25">
+        <f t="shared" si="0"/>
+        <v>28.500000000000007</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="C26">
+        <v>25</v>
+      </c>
+      <c r="D26">
+        <v>7900</v>
+      </c>
+      <c r="J26">
+        <v>73.099999999999994</v>
+      </c>
+      <c r="K26">
+        <v>44.9</v>
+      </c>
+      <c r="L26">
+        <f t="shared" si="0"/>
+        <v>28.199999999999996</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A27" s="1"/>
+      <c r="B27" s="1"/>
+      <c r="C27" s="1">
+        <v>26</v>
+      </c>
+      <c r="D27" s="1">
+        <v>7800</v>
+      </c>
+      <c r="E27" s="1">
+        <v>1.5E-3</v>
+      </c>
+      <c r="F27" s="1">
+        <v>875</v>
+      </c>
+      <c r="G27" s="1">
+        <v>0.218</v>
+      </c>
+      <c r="H27" s="1">
+        <v>1.2E-2</v>
+      </c>
+      <c r="I27" s="1"/>
+      <c r="J27" s="1">
+        <v>72.400000000000006</v>
+      </c>
+      <c r="K27" s="1">
+        <v>44.3</v>
+      </c>
+      <c r="L27" s="1">
+        <f t="shared" si="0"/>
+        <v>28.100000000000009</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A49"/>
       <c r="B49"/>
       <c r="C49"/>
@@ -579,6 +1099,20 @@
       <c r="K49"/>
       <c r="L49"/>
     </row>
+    <row r="50" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A50"/>
+      <c r="B50"/>
+      <c r="C50"/>
+      <c r="D50"/>
+      <c r="E50"/>
+      <c r="F50"/>
+      <c r="G50"/>
+      <c r="H50"/>
+      <c r="I50"/>
+      <c r="J50"/>
+      <c r="K50"/>
+      <c r="L50"/>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -590,8 +1124,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD1CC053-5A22-4998-AEA2-520BDBBCB823}">
   <dimension ref="A1:L30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E33" sqref="E33"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="A30" sqref="A30:H30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -620,10 +1154,10 @@
         <v>2</v>
       </c>
       <c r="E1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" t="s">
         <v>13</v>
-      </c>
-      <c r="F1" t="s">
-        <v>14</v>
       </c>
       <c r="G1" t="s">
         <v>5</v>
@@ -646,7 +1180,7 @@
     </row>
     <row r="2" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>10</v>
@@ -685,7 +1219,7 @@
     </row>
     <row r="3" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>10</v>
@@ -724,7 +1258,7 @@
     </row>
     <row r="4" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>10</v>
@@ -763,7 +1297,7 @@
     </row>
     <row r="5" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>10</v>
@@ -956,7 +1490,7 @@
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A17" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>10</v>
@@ -1217,7 +1751,7 @@
     </row>
     <row r="30" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>10</v>

</xml_diff>

<commit_message>
Pub changes; millennial rerun files
</commit_message>
<xml_diff>
--- a/Millennial/R/simulation/LRF/Calibration tests_LRF.xlsx
+++ b/Millennial/R/simulation/LRF/Calibration tests_LRF.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\edmaas\Documents\Modeling\Millennial\R\simulation\LRF\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alask\Documents\Modeling\Millennial\R\simulation\LRF\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7567018-BF05-4808-BB00-EC5DF371F5C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6633FB07-EB14-44F5-9583-F21AE073687D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34635" yWindow="3780" windowWidth="18540" windowHeight="9765" xr2:uid="{BB3C2B61-1532-46D1-807E-A73843A0FCA4}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{BB3C2B61-1532-46D1-807E-A73843A0FCA4}"/>
   </bookViews>
   <sheets>
     <sheet name="1_3" sheetId="1" r:id="rId1"/>
@@ -104,7 +104,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -131,6 +131,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <strike/>
+      <sz val="11"/>
+      <color theme="9"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -152,10 +160,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -473,23 +482,23 @@
   <dimension ref="A1:M50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I27" sqref="I27"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="N27" sqref="N27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="7.90625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.453125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="4.26953125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.54296875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.54296875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.54296875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.08984375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>8</v>
       </c>
@@ -530,7 +539,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -572,7 +581,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>10</v>
       </c>
@@ -608,7 +617,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>10</v>
       </c>
@@ -644,7 +653,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="C5">
         <v>4</v>
       </c>
@@ -662,7 +671,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="C6">
         <v>5</v>
       </c>
@@ -680,7 +689,7 @@
         <v>29.4</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="C7">
         <v>6</v>
       </c>
@@ -698,7 +707,7 @@
         <v>32.1</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="C8">
         <v>7</v>
       </c>
@@ -716,7 +725,7 @@
         <v>31.299999999999997</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="C9">
         <v>8</v>
       </c>
@@ -734,7 +743,7 @@
         <v>36.9</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="C10">
         <v>9</v>
       </c>
@@ -755,7 +764,7 @@
         <v>41.900000000000006</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="C11">
         <v>10</v>
       </c>
@@ -776,7 +785,7 @@
         <v>42.5</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="C12">
         <v>11</v>
       </c>
@@ -794,7 +803,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="C13">
         <v>12</v>
       </c>
@@ -812,7 +821,7 @@
         <v>45.3</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="C14">
         <v>13</v>
       </c>
@@ -830,7 +839,7 @@
         <v>41.4</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="C15">
         <v>14</v>
       </c>
@@ -848,7 +857,7 @@
         <v>44.300000000000004</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="C16">
         <v>15</v>
       </c>
@@ -866,7 +875,7 @@
         <v>33.400000000000006</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C17">
         <v>16</v>
       </c>
@@ -884,7 +893,7 @@
         <v>26.6</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C18">
         <v>17</v>
       </c>
@@ -902,7 +911,7 @@
         <v>27.1</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C19">
         <v>18</v>
       </c>
@@ -923,7 +932,7 @@
         <v>26.4</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C20">
         <v>19</v>
       </c>
@@ -941,7 +950,7 @@
         <v>33.5</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C21">
         <v>20</v>
       </c>
@@ -959,7 +968,7 @@
         <v>32.999999999999993</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C22">
         <v>21</v>
       </c>
@@ -980,7 +989,7 @@
         <v>26.4</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C23">
         <v>22</v>
       </c>
@@ -998,7 +1007,7 @@
         <v>25.900000000000006</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C24">
         <v>23</v>
       </c>
@@ -1016,7 +1025,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C25">
         <v>24</v>
       </c>
@@ -1034,7 +1043,7 @@
         <v>28.500000000000007</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C26">
         <v>25</v>
       </c>
@@ -1052,7 +1061,7 @@
         <v>28.199999999999996</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1">
@@ -1067,25 +1076,30 @@
       <c r="F27" s="1">
         <v>875</v>
       </c>
-      <c r="G27" s="1">
+      <c r="G27" s="3">
         <v>0.218</v>
       </c>
       <c r="H27" s="1">
         <v>1.2E-2</v>
       </c>
       <c r="I27" s="1"/>
-      <c r="J27" s="1">
+      <c r="J27" s="3">
         <v>72.400000000000006</v>
       </c>
-      <c r="K27" s="1">
+      <c r="K27" s="3">
         <v>44.3</v>
       </c>
-      <c r="L27" s="1">
+      <c r="L27" s="3">
         <f t="shared" si="0"/>
         <v>28.100000000000009</v>
       </c>
     </row>
-    <row r="49" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="G28" s="1">
+        <v>0.216</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A49"/>
       <c r="B49"/>
       <c r="C49"/>
@@ -1099,7 +1113,7 @@
       <c r="K49"/>
       <c r="L49"/>
     </row>
-    <row r="50" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A50"/>
       <c r="B50"/>
       <c r="C50"/>
@@ -1128,19 +1142,19 @@
       <selection activeCell="A30" sqref="A30:H30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="7.90625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.453125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="4.26953125" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="6.54296875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.54296875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.08984375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="5.81640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="5.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="6.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.77734375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="5.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>8</v>
       </c>
@@ -1178,7 +1192,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>11</v>
       </c>
@@ -1217,7 +1231,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="3" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>14</v>
       </c>
@@ -1256,7 +1270,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>14</v>
       </c>
@@ -1295,7 +1309,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>14</v>
       </c>
@@ -1334,7 +1348,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C8">
         <v>0</v>
       </c>
@@ -1366,7 +1380,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C9">
         <v>1</v>
       </c>
@@ -1383,7 +1397,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C10">
         <v>2</v>
       </c>
@@ -1400,7 +1414,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C11">
         <v>3</v>
       </c>
@@ -1420,7 +1434,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C12">
         <v>4</v>
       </c>
@@ -1437,7 +1451,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C13">
         <v>5</v>
       </c>
@@ -1454,7 +1468,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C14">
         <v>6</v>
       </c>
@@ -1471,7 +1485,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C15">
         <v>7</v>
       </c>
@@ -1488,7 +1502,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>14</v>
       </c>
@@ -1527,7 +1541,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C18">
         <v>1</v>
       </c>
@@ -1545,7 +1559,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C19" s="2">
         <v>2</v>
       </c>
@@ -1563,7 +1577,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C20">
         <v>3</v>
       </c>
@@ -1581,7 +1595,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C21" s="2">
         <v>4</v>
       </c>
@@ -1605,7 +1619,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C22">
         <v>5</v>
       </c>
@@ -1623,7 +1637,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C23" s="2">
         <v>6</v>
       </c>
@@ -1641,7 +1655,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C24">
         <v>7</v>
       </c>
@@ -1659,7 +1673,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C25" s="2">
         <v>8</v>
       </c>
@@ -1677,7 +1691,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C26">
         <v>9</v>
       </c>
@@ -1695,7 +1709,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C27" s="2">
         <v>10</v>
       </c>
@@ -1713,7 +1727,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C28">
         <v>11</v>
       </c>
@@ -1731,7 +1745,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C29" s="2">
         <v>12</v>
       </c>
@@ -1749,7 +1763,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="30" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>14</v>
       </c>

</xml_diff>